<commit_message>
FUNCTIONALITY: NextAndBackButtonStates - Corrected the connection path. NextAndBackFunctionality - Finished writing the suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -624,7 +624,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote a new test case.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Timing</t>
+  </si>
+  <si>
+    <t>Encryption</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -172,16 +175,20 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -199,6 +206,35 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <gradientFill>
           <stop position="0">
             <color rgb="FF00B0F0"/>
@@ -213,6 +249,107 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
         </patternFill>
       </fill>
     </dxf>
@@ -530,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,33 +697,33 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$2:A37)</f>
-        <v>2</v>
+        <f>COUNTA($A:$A) -1</f>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$2:D36,"Ready to Write")+COUNTIF($D$2:D36,"Outdated")</f>
-        <v>1</v>
+        <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
+        <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -595,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$2:D36,"Automated")+COUNTIF($D$2:D36,"Finished")</f>
+        <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -610,21 +747,33 @@
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$2:C36)</f>
-        <v>18</v>
+        <f>SUM($C:$C)</f>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -632,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$2:B36)</f>
+        <f>SUM($B:$B)</f>
         <v>0</v>
       </c>
     </row>
@@ -660,32 +809,60 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D50">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="D3:D51">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+      <formula>LEN(TRIM(D3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: IntegrationPointKeywords - Added a decent error message. Read - Began attempting to automate the Test Suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +677,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
@@ -709,7 +709,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote four new test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -607,7 +607,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>16</v>
@@ -715,7 +715,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.4375</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote a pair of new test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -69,7 +69,7 @@
     <t>Finished</t>
   </si>
   <si>
-    <t>Contains two partially automated test cases.</t>
+    <t>Contains four partially automated test cases.</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>16</v>
@@ -715,7 +715,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.55000000000000004</v>
+        <v>0.59090909090909094</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote a few new test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -173,74 +173,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -683,7 +616,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +718,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
@@ -833,7 +766,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.41935483870967744</v>
+        <v>0.37142857142857144</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -852,58 +785,58 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D2:D52">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="14" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed an obsolete test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Read/_Test_Suite_Statistics.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceCode\IntegrationPoints\QA\Tests\CRUD\Read\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="20580" windowHeight="11640"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -70,9 +75,6 @@
   </si>
   <si>
     <t>Contains four partially automated test cases.</t>
-  </si>
-  <si>
-    <t>JobStatus</t>
   </si>
   <si>
     <t>Ready to Write</t>
@@ -322,6 +324,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -369,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -616,7 +621,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,26 +651,26 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -674,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -702,40 +707,43 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -746,27 +754,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.37142857142857144</v>
+        <v>0.44827586206896552</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -784,7 +777,7 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D52">
+  <conditionalFormatting sqref="D2:D51">
     <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>

</xml_diff>